<commit_message>
update cutrun metadata all lines
</commit_message>
<xml_diff>
--- a/GEO/CUT&RUN_PXGL_Primed.xlsx
+++ b/GEO/CUT&RUN_PXGL_Primed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\surfi\Desktop\charbel_paper_github_v1\GEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4290F8-9ECC-4EB1-98CF-0A344545CDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F51699-914F-4BFD-A93B-4612178340C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="874" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5607,7 +5607,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="945">
   <si>
     <t>SAMPLES</t>
   </si>
@@ -9042,66 +9042,6 @@
   </si>
   <si>
     <t>Primed_IgG_Rep2.hg38.BPM.all.bw</t>
-  </si>
-  <si>
-    <t>D725C01.R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C04.R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C05.R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C06.R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C07.R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C08.R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C11.R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C12.R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C13.R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C14.R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C01.R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C04.R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C05.R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C06.R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C07.R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C08.R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C11.R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C12.R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C13.R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>D725C14.R2.fastq.gz</t>
   </si>
   <si>
     <t xml:space="preserve">XIST dampens X chromosome activity in a SPEN-dependent manner during early human development </t>
@@ -9915,6 +9855,18 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -9928,18 +9880,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -9973,7 +9913,47 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
     <cellStyle name="Normal 3" xfId="27" xr:uid="{F4D64B01-3AA2-4CE5-A7EE-64332280C940}"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -14322,30 +14302,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="71" t="s">
         <v>462</v>
       </c>
-      <c r="B1" s="67"/>
+      <c r="B1" s="71"/>
     </row>
     <row r="2" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="74"/>
-      <c r="B2" s="74"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
     </row>
     <row r="3" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="75"/>
+      <c r="B3" s="70"/>
     </row>
     <row r="4" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="72"/>
+      <c r="B4" s="67"/>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="71"/>
-      <c r="B5" s="71"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
     </row>
     <row r="6" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -14442,79 +14422,79 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="72"/>
-      <c r="B17" s="72"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="68" t="s">
+      <c r="A18" s="72" t="s">
         <v>272</v>
       </c>
-      <c r="B18" s="69"/>
+      <c r="B18" s="73"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="74" t="s">
         <v>577</v>
       </c>
-      <c r="B19" s="70"/>
+      <c r="B19" s="74"/>
     </row>
     <row r="20" spans="1:6" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="73" t="s">
+      <c r="A20" s="68" t="s">
         <v>255</v>
       </c>
-      <c r="B20" s="73"/>
+      <c r="B20" s="68"/>
     </row>
     <row r="21" spans="1:6" ht="315" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="73" t="s">
+      <c r="A21" s="68" t="s">
         <v>271</v>
       </c>
-      <c r="B21" s="73"/>
+      <c r="B21" s="68"/>
     </row>
     <row r="22" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="72"/>
-      <c r="B22" s="72"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="67"/>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="72"/>
-      <c r="B24" s="72"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="67"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="72"/>
-      <c r="B25" s="72"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="67"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="72"/>
-      <c r="B26" s="72"/>
+      <c r="A26" s="67"/>
+      <c r="B26" s="67"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="72"/>
-      <c r="B27" s="72"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" location="categories" xr:uid="{D6250736-B96D-4C3E-A39D-F5873CF8B173}"/>
@@ -14923,8 +14903,8 @@
   </sheetPr>
   <dimension ref="A1:W195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126:B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="83.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -15045,7 +15025,7 @@
         <v>361</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>943</v>
+        <v>923</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -15053,7 +15033,7 @@
         <v>362</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>944</v>
+        <v>924</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -15326,10 +15306,10 @@
       </c>
       <c r="N34" s="20"/>
       <c r="O34" s="20" t="s">
-        <v>955</v>
+        <v>935</v>
       </c>
       <c r="P34" s="20" t="s">
-        <v>945</v>
+        <v>925</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="15" x14ac:dyDescent="0.25">
@@ -15365,10 +15345,10 @@
       </c>
       <c r="N35" s="20"/>
       <c r="O35" s="20" t="s">
-        <v>956</v>
+        <v>936</v>
       </c>
       <c r="P35" s="20" t="s">
-        <v>946</v>
+        <v>926</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="15" x14ac:dyDescent="0.25">
@@ -15404,10 +15384,10 @@
       </c>
       <c r="N36" s="20"/>
       <c r="O36" s="20" t="s">
-        <v>957</v>
+        <v>937</v>
       </c>
       <c r="P36" s="20" t="s">
-        <v>947</v>
+        <v>927</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="15" x14ac:dyDescent="0.25">
@@ -15443,10 +15423,10 @@
       </c>
       <c r="N37" s="20"/>
       <c r="O37" s="20" t="s">
-        <v>958</v>
+        <v>938</v>
       </c>
       <c r="P37" s="20" t="s">
-        <v>948</v>
+        <v>928</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="15" x14ac:dyDescent="0.25">
@@ -15482,10 +15462,10 @@
       </c>
       <c r="N38" s="20"/>
       <c r="O38" s="20" t="s">
-        <v>959</v>
+        <v>939</v>
       </c>
       <c r="P38" s="20" t="s">
-        <v>949</v>
+        <v>929</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="15" x14ac:dyDescent="0.25">
@@ -15521,10 +15501,10 @@
       </c>
       <c r="N39" s="20"/>
       <c r="O39" s="20" t="s">
-        <v>960</v>
+        <v>940</v>
       </c>
       <c r="P39" s="20" t="s">
-        <v>950</v>
+        <v>930</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="15" x14ac:dyDescent="0.25">
@@ -15560,10 +15540,10 @@
       </c>
       <c r="N40" s="20"/>
       <c r="O40" s="20" t="s">
-        <v>961</v>
+        <v>941</v>
       </c>
       <c r="P40" s="20" t="s">
-        <v>951</v>
+        <v>931</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="15" x14ac:dyDescent="0.25">
@@ -15599,10 +15579,10 @@
       </c>
       <c r="N41" s="20"/>
       <c r="O41" s="20" t="s">
-        <v>962</v>
+        <v>942</v>
       </c>
       <c r="P41" s="20" t="s">
-        <v>952</v>
+        <v>932</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="15" x14ac:dyDescent="0.25">
@@ -15638,10 +15618,10 @@
       </c>
       <c r="N42" s="20"/>
       <c r="O42" s="20" t="s">
-        <v>963</v>
+        <v>943</v>
       </c>
       <c r="P42" s="20" t="s">
-        <v>953</v>
+        <v>933</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="15" x14ac:dyDescent="0.25">
@@ -15677,10 +15657,10 @@
       </c>
       <c r="N43" s="20"/>
       <c r="O43" s="20" t="s">
-        <v>964</v>
+        <v>944</v>
       </c>
       <c r="P43" s="20" t="s">
-        <v>954</v>
+        <v>934</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="15" x14ac:dyDescent="0.25">
@@ -18559,82 +18539,82 @@
     </row>
     <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126" s="20" t="s">
-        <v>923</v>
+        <v>935</v>
       </c>
       <c r="B126" s="20" t="s">
-        <v>933</v>
+        <v>925</v>
       </c>
     </row>
     <row r="127" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A127" s="20" t="s">
-        <v>924</v>
+        <v>936</v>
       </c>
       <c r="B127" s="20" t="s">
-        <v>934</v>
+        <v>926</v>
       </c>
     </row>
     <row r="128" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A128" s="20" t="s">
-        <v>925</v>
+        <v>937</v>
       </c>
       <c r="B128" s="20" t="s">
-        <v>935</v>
+        <v>927</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="20" t="s">
-        <v>926</v>
+        <v>938</v>
       </c>
       <c r="B129" s="20" t="s">
-        <v>936</v>
+        <v>928</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="20" t="s">
-        <v>927</v>
+        <v>939</v>
       </c>
       <c r="B130" s="20" t="s">
-        <v>937</v>
+        <v>929</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="20" t="s">
-        <v>928</v>
+        <v>940</v>
       </c>
       <c r="B131" s="20" t="s">
-        <v>938</v>
+        <v>930</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="20" t="s">
-        <v>929</v>
+        <v>941</v>
       </c>
       <c r="B132" s="20" t="s">
-        <v>939</v>
+        <v>931</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="20" t="s">
-        <v>930</v>
+        <v>942</v>
       </c>
       <c r="B133" s="20" t="s">
-        <v>940</v>
+        <v>932</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="20" t="s">
-        <v>931</v>
+        <v>943</v>
       </c>
       <c r="B134" s="20" t="s">
-        <v>941</v>
+        <v>933</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="20" t="s">
-        <v>932</v>
+        <v>944</v>
       </c>
       <c r="B135" s="20" t="s">
-        <v>942</v>
+        <v>934</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -19120,46 +19100,49 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0"/>
   <conditionalFormatting sqref="A56:A61 A34:A43">
-    <cfRule type="duplicateValues" dxfId="19" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="59"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A136:B195">
+    <cfRule type="duplicateValues" dxfId="21" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A196:XFD1048576 A79:A103 X104:XFD126 X90:XFD90 C126:W126 Q91:XFD103 C127:XFD195">
+    <cfRule type="duplicateValues" dxfId="20" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:B27 B11:B15">
+    <cfRule type="duplicateValues" dxfId="19" priority="39"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:B61">
+    <cfRule type="duplicateValues" dxfId="18" priority="36"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62:B79">
+    <cfRule type="duplicateValues" dxfId="17" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B80:B85">
+    <cfRule type="duplicateValues" dxfId="16" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B86:B91">
+    <cfRule type="duplicateValues" dxfId="15" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B92:B97">
+    <cfRule type="duplicateValues" dxfId="14" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B98:B103">
+    <cfRule type="duplicateValues" dxfId="13" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B106:B112 B114:B119">
+    <cfRule type="duplicateValues" dxfId="12" priority="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O35:P103">
+    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O34:XFD34 Q35:XFD67">
+    <cfRule type="duplicateValues" dxfId="10" priority="35"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A127:B135">
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A126:B126">
-    <cfRule type="duplicateValues" dxfId="18" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A127:B195">
-    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A196:XFD1048576 A79:A103 X104:XFD126 X90:XFD90 C126:W126 Q91:XFD103 C127:XFD195">
-    <cfRule type="duplicateValues" dxfId="16" priority="32"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17:B27 B11:B15">
-    <cfRule type="duplicateValues" dxfId="15" priority="37"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B34:B61">
-    <cfRule type="duplicateValues" dxfId="14" priority="34"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B62:B79">
-    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B80:B85">
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B86:B91">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B92:B97">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B98:B103">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B106:B112 B114:B119">
-    <cfRule type="duplicateValues" dxfId="8" priority="38"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O35:P103">
-    <cfRule type="duplicateValues" dxfId="7" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O34:XFD34 Q35:XFD67">
-    <cfRule type="duplicateValues" dxfId="6" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="15">
     <dataValidation type="textLength" errorStyle="information" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Your summary seems too short!" error="Please provide a thorough description of the goals and objectives of this study.  A working abstract from the associated manuscript may be suitable.  Include as much text as necessary." prompt="Please provide a thorough description of the goals and objectives of this study.  A working abstract from the associated manuscript may be suitable.  Include as much text as necessary." sqref="B12" xr:uid="{6DD1BA29-F299-4D8E-AF94-669CA4660371}">
@@ -19282,10 +19265,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F7:F12">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13:F18">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="Each sample title should be unique. _x000a_Use biol/tech rep numbers (when _x000a_applicable) to unique the titles. _x000a_For example:_x000a_Muscle, exercised, 60min, biol rep1_x000a_Muscle, exercised, 60min, biol rep2_x000a_" sqref="F7:F18" xr:uid="{E1213116-0C92-4E16-8A25-FA0D7A7C18E0}"/>
@@ -19361,7 +19344,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A9:G1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -26249,13 +26232,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="vq7Iatnd+jE8zxfc8RHY55fRB2dEGEJ3skZO89caxOF1BDbSneErENA/VUKxyZa97CW266clRXMnwj+vpKgg4g==" saltValue="+ZFTuxJiYJiRThwP1ksobg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <conditionalFormatting sqref="A61:E69">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:Y31">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T26:Y31">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from the drop down menu" sqref="I30:K32" xr:uid="{79D6ECAE-44AD-41AB-84C9-88F44BE0AE81}">

</xml_diff>

<commit_message>
update cutrun metadata all lines 2
</commit_message>
<xml_diff>
--- a/GEO/CUT&RUN_PXGL_Primed.xlsx
+++ b/GEO/CUT&RUN_PXGL_Primed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\surfi\Desktop\charbel_paper_github_v1\GEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F51699-914F-4BFD-A93B-4612178340C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DD9D77-B03B-4DB0-B7E7-5AE379E4F525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="874" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,14 +31,6 @@
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -629,7 +621,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q33" authorId="0" shapeId="0" xr:uid="{BD6E6772-95A3-46A2-BD6F-DF0D6C3B1C93}">
+    <comment ref="Q33" authorId="0" shapeId="0" xr:uid="{A2F46A00-3660-40AE-8B06-26B053A91D28}">
       <text>
         <r>
           <rPr>
@@ -645,7 +637,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R33" authorId="0" shapeId="0" xr:uid="{0F60EE06-13E2-4E08-A4F1-5C272396AC26}">
+    <comment ref="R33" authorId="0" shapeId="0" xr:uid="{18A6F91A-F024-47FE-B5D8-DC6805D1A137}">
       <text>
         <r>
           <rPr>
@@ -5607,7 +5599,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2237" uniqueCount="1087">
   <si>
     <t>SAMPLES</t>
   </si>
@@ -9108,6 +9100,432 @@
   </si>
   <si>
     <t>D725C14_trimmed.R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>md5sum_r1</t>
+  </si>
+  <si>
+    <t>md5sum_r2</t>
+  </si>
+  <si>
+    <t>ea46ec2721c09e17963d03d5cb05a731</t>
+  </si>
+  <si>
+    <t>7106766e1854e397c517d42330401e51</t>
+  </si>
+  <si>
+    <t>5fda6b25e0df22f5d217384bac910537</t>
+  </si>
+  <si>
+    <t>43a14b4d47233cef5cb8992b3f472b87</t>
+  </si>
+  <si>
+    <t>83501f0bb2922d83df661d96f2019a2b</t>
+  </si>
+  <si>
+    <t>1c2557b9269a30a5ae75037eebfa08d1</t>
+  </si>
+  <si>
+    <t>a5de2092b4f3b476151c1b2aa3e5c6b4</t>
+  </si>
+  <si>
+    <t>351d1a9c4755b822acff89519779b55b</t>
+  </si>
+  <si>
+    <t>6f260d1d60ed3cbedf80b004cb7ba76e</t>
+  </si>
+  <si>
+    <t>c937a6324e49d75eb64011c77976eb6f</t>
+  </si>
+  <si>
+    <t>cd81380217e808f328d6cbe77f21a510</t>
+  </si>
+  <si>
+    <t>681702907c2c02c72a324179a45b1d23</t>
+  </si>
+  <si>
+    <t>3cce6b50e2dc08ce70c6a1d45334da8e</t>
+  </si>
+  <si>
+    <t>1f385fd5171261efcf737a93a75921a7</t>
+  </si>
+  <si>
+    <t>0bede33a496d5d0e60309fdff1c40ade</t>
+  </si>
+  <si>
+    <t>07503d066fb6ed5c20bb4f5cdef09f9d</t>
+  </si>
+  <si>
+    <t>a204e34edf4479f4cb7e488e0d0b4d8e</t>
+  </si>
+  <si>
+    <t>3a42ca3172ee84841c0afb4b28ea2bd2</t>
+  </si>
+  <si>
+    <t>945619c82056c6bcc5c65f25a2c03f5d</t>
+  </si>
+  <si>
+    <t>c77a3fe249ef536ff948d6a718247376</t>
+  </si>
+  <si>
+    <t>a5e0931c453296d50ebd08c0866bb195</t>
+  </si>
+  <si>
+    <t>91aaebcf9106279fa7f1e7cdd288652d</t>
+  </si>
+  <si>
+    <t>91c9a1de766fca4e7a7fd1078eb8c679</t>
+  </si>
+  <si>
+    <t>5869820efa6971394102aa098b1f7b03</t>
+  </si>
+  <si>
+    <t>067037625d38bcfb5cd54003b0696a6d</t>
+  </si>
+  <si>
+    <t>31ec901861b288dbd1c16ff1c433e0f5</t>
+  </si>
+  <si>
+    <t>f571b4082ffa1ccbc79eed07f8f164a8</t>
+  </si>
+  <si>
+    <t>707e2a0686f0c1f8cedb2948e0551358</t>
+  </si>
+  <si>
+    <t>6e5768023c5c82fa89dfc0a82ab2181e</t>
+  </si>
+  <si>
+    <t>f103a0417e43632126e1b36e4327a93e</t>
+  </si>
+  <si>
+    <t>fa0c8f8f52d8324038e783bd16d61e3a</t>
+  </si>
+  <si>
+    <t>7ee2a10d3a4b7acc76785a89358a3999</t>
+  </si>
+  <si>
+    <t>848a24fe883837576f44643f20cc6c4c</t>
+  </si>
+  <si>
+    <t>e54f9c9a386691b1fcd03304975eecd1</t>
+  </si>
+  <si>
+    <t>b735f2601f2de5bdacb237da3cb08ae1</t>
+  </si>
+  <si>
+    <t>06d7ab6bcf4f98f807eebfbf3873cbc0</t>
+  </si>
+  <si>
+    <t>e2f4df1a27eaa96f5b9c24f156d36118</t>
+  </si>
+  <si>
+    <t>5166ddd573fa7fabe99a30b06685b0aa</t>
+  </si>
+  <si>
+    <t>7688dd4eb4278520c7109eb56a60527b</t>
+  </si>
+  <si>
+    <t>1393d3dcddae99a3d430d4f495985216</t>
+  </si>
+  <si>
+    <t>f96966668e4408ac41ba80f19750cedc</t>
+  </si>
+  <si>
+    <t>0cbb6792ff943e3616cd87661c3f7b7f</t>
+  </si>
+  <si>
+    <t>7b6a97d7fdab45d207127ba08f3c495a</t>
+  </si>
+  <si>
+    <t>7e44db7bc200fa993364e1b7ff2224e4</t>
+  </si>
+  <si>
+    <t>8f0acf71da2c23351b78e50968e47e52</t>
+  </si>
+  <si>
+    <t>f5fff8c760471076345b7822b215f04e</t>
+  </si>
+  <si>
+    <t>8a9ab0bcd2000be74e46e1df9125d2ca</t>
+  </si>
+  <si>
+    <t>e8c8be971365bbed68c023b73c5ca9b8</t>
+  </si>
+  <si>
+    <t>41c0496ed71683fdd7049727573f6c77</t>
+  </si>
+  <si>
+    <t>20066b894ae2140f104748ba1af4eaf6</t>
+  </si>
+  <si>
+    <t>9c983a1be6a359052ad7546298f0d530</t>
+  </si>
+  <si>
+    <t>ecfcb7c0b5cdd7f8fadc38cc4053626e</t>
+  </si>
+  <si>
+    <t>3e0e9fff510a7fe07155a02fc4ece284</t>
+  </si>
+  <si>
+    <t>4ecf657deebc4cce814784ccf06865cf</t>
+  </si>
+  <si>
+    <t>41d4cc0ceca6f9f3e3bb8d0e2ecf4fae</t>
+  </si>
+  <si>
+    <t>d0d0de3a95c0fcb4585f24980b0ce981</t>
+  </si>
+  <si>
+    <t>612c547e96bd0298da374ff5ccf01475</t>
+  </si>
+  <si>
+    <t>aad8097cd9003e0929b7a2b0dadf6d6e</t>
+  </si>
+  <si>
+    <t>d0c8bb410033c2d2dd50b0a0fe2787fc</t>
+  </si>
+  <si>
+    <t>6d07f6408b1f8ff48bc1af4d1bd9fd03</t>
+  </si>
+  <si>
+    <t>39c7794c1f0ec24ccdf11865d69f7550</t>
+  </si>
+  <si>
+    <t>179829f54404ba9c257abb41c0fa9000</t>
+  </si>
+  <si>
+    <t>561b9bb95baad6e1dd4a1c2c98b3c0f6</t>
+  </si>
+  <si>
+    <t>967dc562959c06de5d82f6fbf664b1e8</t>
+  </si>
+  <si>
+    <t>e2de35a32e8e04f4c7eade6104d0204d</t>
+  </si>
+  <si>
+    <t>528048c4a21854f1438d2be4147c540b</t>
+  </si>
+  <si>
+    <t>da02b564fd0f24fe8d843e3839a793f3</t>
+  </si>
+  <si>
+    <t>82426bdd9a734a19fa77b27d89f5cfeb</t>
+  </si>
+  <si>
+    <t>334c5a59582cd2e5f87c3965041c19c0</t>
+  </si>
+  <si>
+    <t>cda39fcd114e81da1251014d31968656</t>
+  </si>
+  <si>
+    <t>19d851346766bcea6739868809b1ec6f</t>
+  </si>
+  <si>
+    <t>ec3363e7421d8e714c6d989a1daaeeac</t>
+  </si>
+  <si>
+    <t>c4915f2d86dce88921acdfebea3acb34</t>
+  </si>
+  <si>
+    <t>da12c6d51eb7b61d7995bef328003388</t>
+  </si>
+  <si>
+    <t>87f3caf13cf954309bec99a9dd173803</t>
+  </si>
+  <si>
+    <t>46256aa85233d87a46a05f383f76b186</t>
+  </si>
+  <si>
+    <t>2aad243e9c470b5f67e84c4ca4bea101</t>
+  </si>
+  <si>
+    <t>aae772dc3c01a2802844b1cd083a3ea8</t>
+  </si>
+  <si>
+    <t>28e085dadb129a5a0ac6dc4641a5dae2</t>
+  </si>
+  <si>
+    <t>2e8ab7d2a90f20b869f7ad5bb11c88fa</t>
+  </si>
+  <si>
+    <t>419c574c2540fd52dc2e3b88f83d9c50</t>
+  </si>
+  <si>
+    <t>6df2acfd72555014f86d920a566c7aff</t>
+  </si>
+  <si>
+    <t>78bd36d6b60196d03f452f4ecc25dedb</t>
+  </si>
+  <si>
+    <t>1e4af588276b782197754552b44e3a57</t>
+  </si>
+  <si>
+    <t>c7475460b3aa1b823ac6d1702e1bb616</t>
+  </si>
+  <si>
+    <t>85301e93cb4facdfba26a0ef80f09a33</t>
+  </si>
+  <si>
+    <t>8898a03e529b615141d88f81f840b1d9</t>
+  </si>
+  <si>
+    <t>30d4871ff059926a49bd7f993fd802ac</t>
+  </si>
+  <si>
+    <t>ecf6ee69adebe64a190cd690cc717b1f</t>
+  </si>
+  <si>
+    <t>de5d1d125bbbbc1a092b80d4f77db23f</t>
+  </si>
+  <si>
+    <t>766db3cde748e11cb9e42cd22b49d5bb</t>
+  </si>
+  <si>
+    <t>00ac9360974707bd9eb8003a78ef0dc2</t>
+  </si>
+  <si>
+    <t>a3900da7d870795a48fdea5b34d55781</t>
+  </si>
+  <si>
+    <t>59a82c1da0f69e6ae7c12b63287eceda</t>
+  </si>
+  <si>
+    <t>79e8c024e0909fbecbf8472716164f55</t>
+  </si>
+  <si>
+    <t>987df3bd2a85642f8374414fb9b21ca4</t>
+  </si>
+  <si>
+    <t>759e34c9c5380bceafb665ed0652764d</t>
+  </si>
+  <si>
+    <t>ccd700a29a9ae03df3e6c08e2ac1c7e7</t>
+  </si>
+  <si>
+    <t>c6d6ab6eb19e7d3ac15b3b5b41da3057</t>
+  </si>
+  <si>
+    <t>cfb781b3aaa5c85bbac2de8422f092c8</t>
+  </si>
+  <si>
+    <t>024959544169174ae7b6cef5e73c6631</t>
+  </si>
+  <si>
+    <t>05d0432ab1ac2b4777245a1aa5862285</t>
+  </si>
+  <si>
+    <t>30cb2a17bc51e5354995118e3a4922ba</t>
+  </si>
+  <si>
+    <t>327f59279e4000709f6db52cff8dac76</t>
+  </si>
+  <si>
+    <t>36721227e84ba5c437fdd2d59154f436</t>
+  </si>
+  <si>
+    <t>ecdabd62e234d93a3c9eddc08719ecad</t>
+  </si>
+  <si>
+    <t>8a589aec8fec88e5885341dd90885c0f</t>
+  </si>
+  <si>
+    <t>956c0006c0a63661d7e7f0c5e5891271</t>
+  </si>
+  <si>
+    <t>4c7c9e80d5f17eee6c9bda8fda9fab13</t>
+  </si>
+  <si>
+    <t>655603eb06f4234e14c22babd5321f31</t>
+  </si>
+  <si>
+    <t>59d989bc01dbe79549a23594c51dbedc</t>
+  </si>
+  <si>
+    <t>f70268cab165ff2b8176da5df6c6ec11</t>
+  </si>
+  <si>
+    <t>5ff820cad735aca7826933f4c9bacb2a</t>
+  </si>
+  <si>
+    <t>59c6682cf5be95b6b4bfeb34130817e0</t>
+  </si>
+  <si>
+    <t>e2960315188551d87b79f1b8edafa72b</t>
+  </si>
+  <si>
+    <t>4272a7b1214895bc8f1d26e2dcdf23a6</t>
+  </si>
+  <si>
+    <t>81fb1f75a85e6caf81e2b3b2a142210c</t>
+  </si>
+  <si>
+    <t>aeba133c7529ca135172c34ea58bd0ae</t>
+  </si>
+  <si>
+    <t>d3721e3cc7f6967d47a0527901dd9747</t>
+  </si>
+  <si>
+    <t>ee2586eda5ac76afcee206b0abdd133b</t>
+  </si>
+  <si>
+    <t>cddd0b8edeef2620b2ac3e872deed6cd</t>
+  </si>
+  <si>
+    <t>43814c5cd7f640029b0027adeac6c7d6</t>
+  </si>
+  <si>
+    <t>188ef5beb334b68421f62b4bab47fac2</t>
+  </si>
+  <si>
+    <t>e178205892124a010fb732d706ac1bf8</t>
+  </si>
+  <si>
+    <t>cdb8a2c0bb6baf499fa329db2bea9fc0</t>
+  </si>
+  <si>
+    <t>e5ea349817c5f31cc81b02eea2743089</t>
+  </si>
+  <si>
+    <t>941dacf1347bcbcbe433e02345e81c27</t>
+  </si>
+  <si>
+    <t>9db2b7bd733b52b32cc43cbfaa3e0802</t>
+  </si>
+  <si>
+    <t>a309bb69fe6989f4ebac0eb57fcb6297</t>
+  </si>
+  <si>
+    <t>1f57d1369151108a8efdeb38cd1d0d81</t>
+  </si>
+  <si>
+    <t>e562208c84e916491d1330b911af67b2</t>
+  </si>
+  <si>
+    <t>dc06233c7f49de9f2ac70db25c5d491c</t>
+  </si>
+  <si>
+    <t>97b27025e989677dc2abfce3303b6992</t>
+  </si>
+  <si>
+    <t>e9fd6215c4db16f6254b6fa291cb2965</t>
+  </si>
+  <si>
+    <t>ed3a3b565518d036d7e9c08179248c5a</t>
+  </si>
+  <si>
+    <t>d2ab61da4ec10e47094a15b479004663</t>
+  </si>
+  <si>
+    <t>b3818a96bc828fbc7571224fbf49732d</t>
+  </si>
+  <si>
+    <t>27e59e81d49a54928d2a89cdc7458400</t>
+  </si>
+  <si>
+    <t>87b1f22daad9fbbd5d263953aeba820f</t>
+  </si>
+  <si>
+    <t>add25fdb2403d4fa4811adfd6f3e7706</t>
   </si>
 </sst>
 </file>
@@ -9661,7 +10079,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -9882,6 +10300,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="11" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="40 % - Accent1" xfId="3" builtinId="31"/>
@@ -9913,37 +10334,7 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
     <cellStyle name="Normal 3" xfId="27" xr:uid="{F4D64B01-3AA2-4CE5-A7EE-64332280C940}"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -14903,8 +15294,8 @@
   </sheetPr>
   <dimension ref="A1:W195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126:B135"/>
+    <sheetView tabSelected="1" topLeftCell="B48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q103" sqref="Q103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="83.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -15267,18 +15658,18 @@
         <v>3</v>
       </c>
       <c r="Q33" s="37" t="s">
-        <v>3</v>
+        <v>945</v>
       </c>
       <c r="R33" s="37" t="s">
-        <v>3</v>
+        <v>946</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>583</v>
+        <v>630</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>593</v>
+        <v>663</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>578</v>
@@ -15302,22 +15693,28 @@
       </c>
       <c r="L34" s="20"/>
       <c r="M34" s="20" t="s">
-        <v>913</v>
+        <v>853</v>
       </c>
       <c r="N34" s="20"/>
       <c r="O34" s="20" t="s">
-        <v>935</v>
+        <v>733</v>
       </c>
       <c r="P34" s="20" t="s">
-        <v>925</v>
+        <v>793</v>
+      </c>
+      <c r="Q34" s="14" t="s">
+        <v>1006</v>
+      </c>
+      <c r="R34" s="14" t="s">
+        <v>1007</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>584</v>
+        <v>627</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>594</v>
+        <v>664</v>
       </c>
       <c r="C35" s="20" t="s">
         <v>578</v>
@@ -15341,22 +15738,28 @@
       </c>
       <c r="L35" s="20"/>
       <c r="M35" s="20" t="s">
-        <v>914</v>
+        <v>854</v>
       </c>
       <c r="N35" s="20"/>
       <c r="O35" s="20" t="s">
-        <v>936</v>
+        <v>734</v>
       </c>
       <c r="P35" s="20" t="s">
-        <v>926</v>
+        <v>794</v>
+      </c>
+      <c r="Q35" s="14" t="s">
+        <v>947</v>
+      </c>
+      <c r="R35" s="14" t="s">
+        <v>1018</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>585</v>
+        <v>628</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>595</v>
+        <v>665</v>
       </c>
       <c r="C36" s="20" t="s">
         <v>578</v>
@@ -15380,22 +15783,28 @@
       </c>
       <c r="L36" s="20"/>
       <c r="M36" s="20" t="s">
-        <v>915</v>
+        <v>855</v>
       </c>
       <c r="N36" s="20"/>
       <c r="O36" s="20" t="s">
-        <v>937</v>
+        <v>735</v>
       </c>
       <c r="P36" s="20" t="s">
-        <v>927</v>
+        <v>795</v>
+      </c>
+      <c r="Q36" s="76" t="s">
+        <v>948</v>
+      </c>
+      <c r="R36" s="14" t="s">
+        <v>1019</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>586</v>
+        <v>629</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>596</v>
+        <v>666</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>578</v>
@@ -15419,22 +15828,28 @@
       </c>
       <c r="L37" s="20"/>
       <c r="M37" s="20" t="s">
-        <v>916</v>
+        <v>856</v>
       </c>
       <c r="N37" s="20"/>
       <c r="O37" s="20" t="s">
-        <v>938</v>
+        <v>736</v>
       </c>
       <c r="P37" s="20" t="s">
-        <v>928</v>
+        <v>796</v>
+      </c>
+      <c r="Q37" s="14" t="s">
+        <v>949</v>
+      </c>
+      <c r="R37" s="14" t="s">
+        <v>1020</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>587</v>
+        <v>659</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>597</v>
+        <v>667</v>
       </c>
       <c r="C38" s="20" t="s">
         <v>578</v>
@@ -15458,22 +15873,28 @@
       </c>
       <c r="L38" s="20"/>
       <c r="M38" s="20" t="s">
-        <v>917</v>
+        <v>857</v>
       </c>
       <c r="N38" s="20"/>
       <c r="O38" s="20" t="s">
-        <v>939</v>
+        <v>737</v>
       </c>
       <c r="P38" s="20" t="s">
-        <v>929</v>
+        <v>797</v>
+      </c>
+      <c r="Q38" s="14" t="s">
+        <v>950</v>
+      </c>
+      <c r="R38" s="14" t="s">
+        <v>1021</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>588</v>
+        <v>660</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>598</v>
+        <v>668</v>
       </c>
       <c r="C39" s="20" t="s">
         <v>578</v>
@@ -15497,22 +15918,28 @@
       </c>
       <c r="L39" s="20"/>
       <c r="M39" s="20" t="s">
-        <v>918</v>
+        <v>858</v>
       </c>
       <c r="N39" s="20"/>
       <c r="O39" s="20" t="s">
-        <v>940</v>
+        <v>738</v>
       </c>
       <c r="P39" s="20" t="s">
-        <v>930</v>
+        <v>798</v>
+      </c>
+      <c r="Q39" s="14" t="s">
+        <v>951</v>
+      </c>
+      <c r="R39" s="14" t="s">
+        <v>1022</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>589</v>
+        <v>661</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>599</v>
+        <v>669</v>
       </c>
       <c r="C40" s="20" t="s">
         <v>578</v>
@@ -15536,22 +15963,28 @@
       </c>
       <c r="L40" s="20"/>
       <c r="M40" s="20" t="s">
-        <v>919</v>
+        <v>859</v>
       </c>
       <c r="N40" s="20"/>
       <c r="O40" s="20" t="s">
-        <v>941</v>
+        <v>739</v>
       </c>
       <c r="P40" s="20" t="s">
-        <v>931</v>
+        <v>799</v>
+      </c>
+      <c r="Q40" s="14" t="s">
+        <v>952</v>
+      </c>
+      <c r="R40" s="14" t="s">
+        <v>1023</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>590</v>
+        <v>662</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>600</v>
+        <v>670</v>
       </c>
       <c r="C41" s="20" t="s">
         <v>578</v>
@@ -15575,22 +16008,28 @@
       </c>
       <c r="L41" s="20"/>
       <c r="M41" s="20" t="s">
-        <v>920</v>
+        <v>860</v>
       </c>
       <c r="N41" s="20"/>
       <c r="O41" s="20" t="s">
-        <v>942</v>
+        <v>740</v>
       </c>
       <c r="P41" s="20" t="s">
-        <v>932</v>
+        <v>800</v>
+      </c>
+      <c r="Q41" s="14" t="s">
+        <v>953</v>
+      </c>
+      <c r="R41" s="14" t="s">
+        <v>1024</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>591</v>
+        <v>631</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>601</v>
+        <v>671</v>
       </c>
       <c r="C42" s="20" t="s">
         <v>578</v>
@@ -15614,22 +16053,28 @@
       </c>
       <c r="L42" s="20"/>
       <c r="M42" s="20" t="s">
-        <v>921</v>
+        <v>861</v>
       </c>
       <c r="N42" s="20"/>
       <c r="O42" s="20" t="s">
-        <v>943</v>
+        <v>741</v>
       </c>
       <c r="P42" s="20" t="s">
-        <v>933</v>
+        <v>801</v>
+      </c>
+      <c r="Q42" s="14" t="s">
+        <v>954</v>
+      </c>
+      <c r="R42" s="14" t="s">
+        <v>1025</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>592</v>
+        <v>632</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>602</v>
+        <v>672</v>
       </c>
       <c r="C43" s="20" t="s">
         <v>578</v>
@@ -15653,22 +16098,28 @@
       </c>
       <c r="L43" s="20"/>
       <c r="M43" s="20" t="s">
-        <v>922</v>
+        <v>862</v>
       </c>
       <c r="N43" s="20"/>
       <c r="O43" s="20" t="s">
-        <v>944</v>
+        <v>742</v>
       </c>
       <c r="P43" s="20" t="s">
-        <v>934</v>
+        <v>802</v>
+      </c>
+      <c r="Q43" s="14" t="s">
+        <v>955</v>
+      </c>
+      <c r="R43" s="14" t="s">
+        <v>1026</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>663</v>
+        <v>673</v>
       </c>
       <c r="C44" s="20" t="s">
         <v>578</v>
@@ -15692,22 +16143,28 @@
       </c>
       <c r="L44" s="20"/>
       <c r="M44" s="20" t="s">
-        <v>853</v>
+        <v>863</v>
       </c>
       <c r="N44" s="20"/>
       <c r="O44" s="20" t="s">
-        <v>733</v>
+        <v>743</v>
       </c>
       <c r="P44" s="20" t="s">
-        <v>793</v>
+        <v>803</v>
+      </c>
+      <c r="Q44" s="14" t="s">
+        <v>956</v>
+      </c>
+      <c r="R44" s="14" t="s">
+        <v>1027</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>627</v>
+        <v>634</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>664</v>
+        <v>674</v>
       </c>
       <c r="C45" s="20" t="s">
         <v>578</v>
@@ -15731,22 +16188,28 @@
       </c>
       <c r="L45" s="20"/>
       <c r="M45" s="20" t="s">
-        <v>854</v>
+        <v>864</v>
       </c>
       <c r="N45" s="20"/>
       <c r="O45" s="20" t="s">
-        <v>734</v>
+        <v>744</v>
       </c>
       <c r="P45" s="20" t="s">
-        <v>794</v>
+        <v>804</v>
+      </c>
+      <c r="Q45" s="14" t="s">
+        <v>957</v>
+      </c>
+      <c r="R45" s="14" t="s">
+        <v>1028</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>628</v>
+        <v>635</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>665</v>
+        <v>675</v>
       </c>
       <c r="C46" s="20" t="s">
         <v>578</v>
@@ -15770,22 +16233,28 @@
       </c>
       <c r="L46" s="20"/>
       <c r="M46" s="20" t="s">
-        <v>855</v>
+        <v>865</v>
       </c>
       <c r="N46" s="20"/>
       <c r="O46" s="20" t="s">
-        <v>735</v>
+        <v>745</v>
       </c>
       <c r="P46" s="20" t="s">
-        <v>795</v>
+        <v>805</v>
+      </c>
+      <c r="Q46" s="14" t="s">
+        <v>958</v>
+      </c>
+      <c r="R46" s="14" t="s">
+        <v>1029</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>629</v>
+        <v>636</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>666</v>
+        <v>676</v>
       </c>
       <c r="C47" s="20" t="s">
         <v>578</v>
@@ -15809,22 +16278,28 @@
       </c>
       <c r="L47" s="20"/>
       <c r="M47" s="20" t="s">
-        <v>856</v>
+        <v>866</v>
       </c>
       <c r="N47" s="20"/>
       <c r="O47" s="20" t="s">
-        <v>736</v>
+        <v>746</v>
       </c>
       <c r="P47" s="20" t="s">
-        <v>796</v>
+        <v>806</v>
+      </c>
+      <c r="Q47" s="14" t="s">
+        <v>959</v>
+      </c>
+      <c r="R47" s="14" t="s">
+        <v>1030</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>659</v>
+        <v>637</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="C48" s="20" t="s">
         <v>578</v>
@@ -15848,22 +16323,28 @@
       </c>
       <c r="L48" s="20"/>
       <c r="M48" s="20" t="s">
-        <v>857</v>
+        <v>867</v>
       </c>
       <c r="N48" s="20"/>
       <c r="O48" s="20" t="s">
-        <v>737</v>
+        <v>747</v>
       </c>
       <c r="P48" s="20" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>807</v>
+      </c>
+      <c r="Q48" s="14" t="s">
+        <v>960</v>
+      </c>
+      <c r="R48" s="14" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>660</v>
+        <v>638</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>668</v>
+        <v>678</v>
       </c>
       <c r="C49" s="20" t="s">
         <v>578</v>
@@ -15887,22 +16368,28 @@
       </c>
       <c r="L49" s="20"/>
       <c r="M49" s="20" t="s">
-        <v>858</v>
+        <v>868</v>
       </c>
       <c r="N49" s="20"/>
       <c r="O49" s="20" t="s">
-        <v>738</v>
+        <v>748</v>
       </c>
       <c r="P49" s="20" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>808</v>
+      </c>
+      <c r="Q49" s="14" t="s">
+        <v>961</v>
+      </c>
+      <c r="R49" s="14" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>661</v>
+        <v>639</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>669</v>
+        <v>679</v>
       </c>
       <c r="C50" s="20" t="s">
         <v>578</v>
@@ -15926,22 +16413,28 @@
       </c>
       <c r="L50" s="20"/>
       <c r="M50" s="20" t="s">
-        <v>859</v>
+        <v>869</v>
       </c>
       <c r="N50" s="20"/>
       <c r="O50" s="20" t="s">
-        <v>739</v>
+        <v>749</v>
       </c>
       <c r="P50" s="20" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>809</v>
+      </c>
+      <c r="Q50" s="14" t="s">
+        <v>962</v>
+      </c>
+      <c r="R50" s="14" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>662</v>
+        <v>640</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>670</v>
+        <v>680</v>
       </c>
       <c r="C51" s="20" t="s">
         <v>578</v>
@@ -15965,22 +16458,28 @@
       </c>
       <c r="L51" s="20"/>
       <c r="M51" s="20" t="s">
-        <v>860</v>
+        <v>870</v>
       </c>
       <c r="N51" s="20"/>
       <c r="O51" s="20" t="s">
-        <v>740</v>
+        <v>750</v>
       </c>
       <c r="P51" s="20" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>810</v>
+      </c>
+      <c r="Q51" s="14" t="s">
+        <v>963</v>
+      </c>
+      <c r="R51" s="14" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>631</v>
+        <v>641</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>671</v>
+        <v>681</v>
       </c>
       <c r="C52" s="20" t="s">
         <v>578</v>
@@ -16004,22 +16503,28 @@
       </c>
       <c r="L52" s="20"/>
       <c r="M52" s="20" t="s">
-        <v>861</v>
+        <v>871</v>
       </c>
       <c r="N52" s="20"/>
       <c r="O52" s="20" t="s">
-        <v>741</v>
+        <v>751</v>
       </c>
       <c r="P52" s="20" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>811</v>
+      </c>
+      <c r="Q52" s="14" t="s">
+        <v>964</v>
+      </c>
+      <c r="R52" s="14" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>632</v>
+        <v>642</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>672</v>
+        <v>682</v>
       </c>
       <c r="C53" s="20" t="s">
         <v>578</v>
@@ -16043,22 +16548,28 @@
       </c>
       <c r="L53" s="20"/>
       <c r="M53" s="20" t="s">
-        <v>862</v>
+        <v>872</v>
       </c>
       <c r="N53" s="20"/>
       <c r="O53" s="20" t="s">
-        <v>742</v>
+        <v>752</v>
       </c>
       <c r="P53" s="20" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>812</v>
+      </c>
+      <c r="Q53" s="14" t="s">
+        <v>965</v>
+      </c>
+      <c r="R53" s="14" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>633</v>
+        <v>643</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>673</v>
+        <v>683</v>
       </c>
       <c r="C54" s="20" t="s">
         <v>578</v>
@@ -16082,22 +16593,28 @@
       </c>
       <c r="L54" s="20"/>
       <c r="M54" s="20" t="s">
-        <v>863</v>
+        <v>873</v>
       </c>
       <c r="N54" s="20"/>
       <c r="O54" s="20" t="s">
-        <v>743</v>
+        <v>753</v>
       </c>
       <c r="P54" s="20" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>813</v>
+      </c>
+      <c r="Q54" s="14" t="s">
+        <v>966</v>
+      </c>
+      <c r="R54" s="14" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>634</v>
+        <v>644</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>674</v>
+        <v>684</v>
       </c>
       <c r="C55" s="20" t="s">
         <v>578</v>
@@ -16121,22 +16638,28 @@
       </c>
       <c r="L55" s="20"/>
       <c r="M55" s="20" t="s">
-        <v>864</v>
+        <v>874</v>
       </c>
       <c r="N55" s="20"/>
       <c r="O55" s="20" t="s">
-        <v>744</v>
+        <v>754</v>
       </c>
       <c r="P55" s="20" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>814</v>
+      </c>
+      <c r="Q55" s="14" t="s">
+        <v>967</v>
+      </c>
+      <c r="R55" s="14" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>635</v>
+        <v>645</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>675</v>
+        <v>685</v>
       </c>
       <c r="C56" s="20" t="s">
         <v>578</v>
@@ -16160,22 +16683,28 @@
       </c>
       <c r="L56" s="20"/>
       <c r="M56" s="20" t="s">
-        <v>865</v>
+        <v>875</v>
       </c>
       <c r="N56" s="20"/>
       <c r="O56" s="20" t="s">
-        <v>745</v>
+        <v>755</v>
       </c>
       <c r="P56" s="20" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>815</v>
+      </c>
+      <c r="Q56" s="14" t="s">
+        <v>968</v>
+      </c>
+      <c r="R56" s="14" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>636</v>
+        <v>646</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>676</v>
+        <v>686</v>
       </c>
       <c r="C57" s="20" t="s">
         <v>578</v>
@@ -16199,26 +16728,33 @@
       </c>
       <c r="L57" s="20"/>
       <c r="M57" s="20" t="s">
-        <v>866</v>
+        <v>876</v>
       </c>
       <c r="N57" s="20"/>
       <c r="O57" s="20" t="s">
-        <v>746</v>
+        <v>756</v>
       </c>
       <c r="P57" s="20" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>816</v>
+      </c>
+      <c r="Q57" s="14" t="s">
+        <v>969</v>
+      </c>
+      <c r="R57" s="14" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>637</v>
+        <v>647</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>677</v>
+        <v>687</v>
       </c>
       <c r="C58" s="20" t="s">
         <v>578</v>
       </c>
+      <c r="D58" s="14"/>
       <c r="E58" s="20" t="s">
         <v>579</v>
       </c>
@@ -16238,26 +16774,33 @@
       </c>
       <c r="L58" s="20"/>
       <c r="M58" s="20" t="s">
-        <v>867</v>
+        <v>877</v>
       </c>
       <c r="N58" s="20"/>
       <c r="O58" s="20" t="s">
-        <v>747</v>
+        <v>757</v>
       </c>
       <c r="P58" s="20" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>817</v>
+      </c>
+      <c r="Q58" s="32" t="s">
+        <v>970</v>
+      </c>
+      <c r="R58" s="32" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>638</v>
+        <v>648</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>678</v>
+        <v>688</v>
       </c>
       <c r="C59" s="20" t="s">
         <v>578</v>
       </c>
+      <c r="D59" s="14"/>
       <c r="E59" s="20" t="s">
         <v>579</v>
       </c>
@@ -16277,22 +16820,33 @@
       </c>
       <c r="L59" s="20"/>
       <c r="M59" s="20" t="s">
-        <v>868</v>
+        <v>878</v>
       </c>
       <c r="N59" s="20"/>
       <c r="O59" s="20" t="s">
-        <v>748</v>
+        <v>758</v>
       </c>
       <c r="P59" s="20" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>818</v>
+      </c>
+      <c r="Q59" s="65" t="s">
+        <v>971</v>
+      </c>
+      <c r="R59" s="65" t="s">
+        <v>1042</v>
+      </c>
+      <c r="S59" s="65"/>
+      <c r="T59" s="65"/>
+      <c r="U59" s="65"/>
+      <c r="V59" s="65"/>
+      <c r="W59" s="65"/>
+    </row>
+    <row r="60" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>639</v>
+        <v>649</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>679</v>
+        <v>689</v>
       </c>
       <c r="C60" s="20" t="s">
         <v>578</v>
@@ -16316,22 +16870,28 @@
       </c>
       <c r="L60" s="20"/>
       <c r="M60" s="20" t="s">
-        <v>869</v>
+        <v>879</v>
       </c>
       <c r="N60" s="20"/>
       <c r="O60" s="20" t="s">
-        <v>749</v>
+        <v>759</v>
       </c>
       <c r="P60" s="20" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>819</v>
+      </c>
+      <c r="Q60" s="14" t="s">
+        <v>972</v>
+      </c>
+      <c r="R60" s="14" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>640</v>
+        <v>650</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>680</v>
+        <v>690</v>
       </c>
       <c r="C61" s="20" t="s">
         <v>578</v>
@@ -16355,22 +16915,28 @@
       </c>
       <c r="L61" s="20"/>
       <c r="M61" s="20" t="s">
-        <v>870</v>
+        <v>880</v>
       </c>
       <c r="N61" s="20"/>
       <c r="O61" s="20" t="s">
-        <v>750</v>
+        <v>760</v>
       </c>
       <c r="P61" s="20" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>820</v>
+      </c>
+      <c r="Q61" s="14" t="s">
+        <v>973</v>
+      </c>
+      <c r="R61" s="14" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>641</v>
+        <v>651</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>681</v>
+        <v>691</v>
       </c>
       <c r="C62" s="20" t="s">
         <v>578</v>
@@ -16394,22 +16960,28 @@
       </c>
       <c r="L62" s="20"/>
       <c r="M62" s="20" t="s">
-        <v>871</v>
+        <v>881</v>
       </c>
       <c r="N62" s="20"/>
       <c r="O62" s="20" t="s">
-        <v>751</v>
+        <v>761</v>
       </c>
       <c r="P62" s="20" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>821</v>
+      </c>
+      <c r="Q62" s="14" t="s">
+        <v>974</v>
+      </c>
+      <c r="R62" s="14" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>642</v>
+        <v>652</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>682</v>
+        <v>692</v>
       </c>
       <c r="C63" s="20" t="s">
         <v>578</v>
@@ -16433,22 +17005,28 @@
       </c>
       <c r="L63" s="20"/>
       <c r="M63" s="20" t="s">
-        <v>872</v>
+        <v>882</v>
       </c>
       <c r="N63" s="20"/>
       <c r="O63" s="20" t="s">
-        <v>752</v>
+        <v>762</v>
       </c>
       <c r="P63" s="20" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>822</v>
+      </c>
+      <c r="Q63" s="76" t="s">
+        <v>975</v>
+      </c>
+      <c r="R63" s="14" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>643</v>
+        <v>653</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>683</v>
+        <v>693</v>
       </c>
       <c r="C64" s="20" t="s">
         <v>578</v>
@@ -16472,22 +17050,28 @@
       </c>
       <c r="L64" s="20"/>
       <c r="M64" s="20" t="s">
-        <v>873</v>
+        <v>883</v>
       </c>
       <c r="N64" s="20"/>
       <c r="O64" s="20" t="s">
-        <v>753</v>
+        <v>763</v>
       </c>
       <c r="P64" s="20" t="s">
-        <v>813</v>
+        <v>823</v>
+      </c>
+      <c r="Q64" s="14" t="s">
+        <v>976</v>
+      </c>
+      <c r="R64" s="14" t="s">
+        <v>1047</v>
       </c>
     </row>
     <row r="65" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>684</v>
+        <v>694</v>
       </c>
       <c r="C65" s="20" t="s">
         <v>578</v>
@@ -16511,22 +17095,28 @@
       </c>
       <c r="L65" s="20"/>
       <c r="M65" s="20" t="s">
-        <v>874</v>
+        <v>884</v>
       </c>
       <c r="N65" s="20"/>
       <c r="O65" s="20" t="s">
-        <v>754</v>
+        <v>764</v>
       </c>
       <c r="P65" s="20" t="s">
-        <v>814</v>
+        <v>824</v>
+      </c>
+      <c r="Q65" s="14" t="s">
+        <v>977</v>
+      </c>
+      <c r="R65" s="14" t="s">
+        <v>1048</v>
       </c>
     </row>
     <row r="66" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>645</v>
+        <v>655</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>685</v>
+        <v>695</v>
       </c>
       <c r="C66" s="20" t="s">
         <v>578</v>
@@ -16550,22 +17140,28 @@
       </c>
       <c r="L66" s="20"/>
       <c r="M66" s="20" t="s">
-        <v>875</v>
+        <v>885</v>
       </c>
       <c r="N66" s="20"/>
       <c r="O66" s="20" t="s">
-        <v>755</v>
+        <v>765</v>
       </c>
       <c r="P66" s="20" t="s">
-        <v>815</v>
+        <v>825</v>
+      </c>
+      <c r="Q66" s="14" t="s">
+        <v>978</v>
+      </c>
+      <c r="R66" s="14" t="s">
+        <v>1049</v>
       </c>
     </row>
     <row r="67" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>646</v>
+        <v>656</v>
       </c>
       <c r="B67" s="20" t="s">
-        <v>686</v>
+        <v>696</v>
       </c>
       <c r="C67" s="20" t="s">
         <v>578</v>
@@ -16589,27 +17185,32 @@
       </c>
       <c r="L67" s="20"/>
       <c r="M67" s="20" t="s">
-        <v>876</v>
+        <v>886</v>
       </c>
       <c r="N67" s="20"/>
       <c r="O67" s="20" t="s">
-        <v>756</v>
+        <v>766</v>
       </c>
       <c r="P67" s="20" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="68" spans="1:23" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>826</v>
+      </c>
+      <c r="Q67" s="14" t="s">
+        <v>979</v>
+      </c>
+      <c r="R67" s="14" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>687</v>
+        <v>697</v>
       </c>
       <c r="C68" s="20" t="s">
         <v>578</v>
       </c>
-      <c r="D68" s="14"/>
       <c r="E68" s="20" t="s">
         <v>579</v>
       </c>
@@ -16629,27 +17230,32 @@
       </c>
       <c r="L68" s="20"/>
       <c r="M68" s="20" t="s">
-        <v>877</v>
+        <v>887</v>
       </c>
       <c r="N68" s="20"/>
       <c r="O68" s="20" t="s">
-        <v>757</v>
+        <v>767</v>
       </c>
       <c r="P68" s="20" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="69" spans="1:23" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>827</v>
+      </c>
+      <c r="Q68" s="14" t="s">
+        <v>980</v>
+      </c>
+      <c r="R68" s="14" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>648</v>
+        <v>658</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>688</v>
+        <v>698</v>
       </c>
       <c r="C69" s="20" t="s">
         <v>578</v>
       </c>
-      <c r="D69" s="14"/>
       <c r="E69" s="20" t="s">
         <v>579</v>
       </c>
@@ -16669,29 +17275,28 @@
       </c>
       <c r="L69" s="20"/>
       <c r="M69" s="20" t="s">
-        <v>878</v>
+        <v>888</v>
       </c>
       <c r="N69" s="20"/>
       <c r="O69" s="20" t="s">
-        <v>758</v>
+        <v>768</v>
       </c>
       <c r="P69" s="20" t="s">
-        <v>818</v>
-      </c>
-      <c r="Q69" s="65"/>
-      <c r="R69" s="65"/>
-      <c r="S69" s="65"/>
-      <c r="T69" s="65"/>
-      <c r="U69" s="65"/>
-      <c r="V69" s="65"/>
-      <c r="W69" s="65"/>
+        <v>828</v>
+      </c>
+      <c r="Q69" s="14" t="s">
+        <v>981</v>
+      </c>
+      <c r="R69" s="14" t="s">
+        <v>1052</v>
+      </c>
     </row>
     <row r="70" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>649</v>
+        <v>603</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>689</v>
+        <v>699</v>
       </c>
       <c r="C70" s="20" t="s">
         <v>578</v>
@@ -16715,22 +17320,28 @@
       </c>
       <c r="L70" s="20"/>
       <c r="M70" s="20" t="s">
-        <v>879</v>
+        <v>889</v>
       </c>
       <c r="N70" s="20"/>
       <c r="O70" s="20" t="s">
-        <v>759</v>
+        <v>769</v>
       </c>
       <c r="P70" s="20" t="s">
-        <v>819</v>
+        <v>829</v>
+      </c>
+      <c r="Q70" s="14" t="s">
+        <v>982</v>
+      </c>
+      <c r="R70" s="14" t="s">
+        <v>1053</v>
       </c>
     </row>
     <row r="71" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>650</v>
+        <v>604</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>690</v>
+        <v>700</v>
       </c>
       <c r="C71" s="20" t="s">
         <v>578</v>
@@ -16754,22 +17365,28 @@
       </c>
       <c r="L71" s="20"/>
       <c r="M71" s="20" t="s">
-        <v>880</v>
+        <v>890</v>
       </c>
       <c r="N71" s="20"/>
       <c r="O71" s="20" t="s">
-        <v>760</v>
+        <v>770</v>
       </c>
       <c r="P71" s="20" t="s">
-        <v>820</v>
+        <v>830</v>
+      </c>
+      <c r="Q71" s="14" t="s">
+        <v>983</v>
+      </c>
+      <c r="R71" s="14" t="s">
+        <v>1054</v>
       </c>
     </row>
     <row r="72" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>651</v>
+        <v>605</v>
       </c>
       <c r="B72" s="20" t="s">
-        <v>691</v>
+        <v>701</v>
       </c>
       <c r="C72" s="20" t="s">
         <v>578</v>
@@ -16793,22 +17410,28 @@
       </c>
       <c r="L72" s="20"/>
       <c r="M72" s="20" t="s">
-        <v>881</v>
+        <v>891</v>
       </c>
       <c r="N72" s="20"/>
       <c r="O72" s="20" t="s">
-        <v>761</v>
+        <v>771</v>
       </c>
       <c r="P72" s="20" t="s">
-        <v>821</v>
+        <v>831</v>
+      </c>
+      <c r="Q72" s="14" t="s">
+        <v>984</v>
+      </c>
+      <c r="R72" s="14" t="s">
+        <v>1055</v>
       </c>
     </row>
     <row r="73" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>652</v>
+        <v>606</v>
       </c>
       <c r="B73" s="20" t="s">
-        <v>692</v>
+        <v>702</v>
       </c>
       <c r="C73" s="20" t="s">
         <v>578</v>
@@ -16832,22 +17455,28 @@
       </c>
       <c r="L73" s="20"/>
       <c r="M73" s="20" t="s">
-        <v>882</v>
+        <v>892</v>
       </c>
       <c r="N73" s="20"/>
       <c r="O73" s="20" t="s">
-        <v>762</v>
+        <v>772</v>
       </c>
       <c r="P73" s="20" t="s">
-        <v>822</v>
+        <v>832</v>
+      </c>
+      <c r="Q73" s="14" t="s">
+        <v>985</v>
+      </c>
+      <c r="R73" s="14" t="s">
+        <v>1056</v>
       </c>
     </row>
     <row r="74" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>653</v>
+        <v>607</v>
       </c>
       <c r="B74" s="20" t="s">
-        <v>693</v>
+        <v>703</v>
       </c>
       <c r="C74" s="20" t="s">
         <v>578</v>
@@ -16871,26 +17500,33 @@
       </c>
       <c r="L74" s="20"/>
       <c r="M74" s="20" t="s">
-        <v>883</v>
+        <v>893</v>
       </c>
       <c r="N74" s="20"/>
       <c r="O74" s="20" t="s">
-        <v>763</v>
+        <v>773</v>
       </c>
       <c r="P74" s="20" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="75" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>833</v>
+      </c>
+      <c r="Q74" s="14" t="s">
+        <v>986</v>
+      </c>
+      <c r="R74" s="14" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>654</v>
+        <v>608</v>
       </c>
       <c r="B75" s="20" t="s">
-        <v>694</v>
+        <v>704</v>
       </c>
       <c r="C75" s="20" t="s">
         <v>578</v>
       </c>
+      <c r="D75" s="14"/>
       <c r="E75" s="20" t="s">
         <v>579</v>
       </c>
@@ -16910,26 +17546,33 @@
       </c>
       <c r="L75" s="20"/>
       <c r="M75" s="20" t="s">
-        <v>884</v>
+        <v>894</v>
       </c>
       <c r="N75" s="20"/>
       <c r="O75" s="20" t="s">
-        <v>764</v>
+        <v>774</v>
       </c>
       <c r="P75" s="20" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="76" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>834</v>
+      </c>
+      <c r="Q75" s="32" t="s">
+        <v>987</v>
+      </c>
+      <c r="R75" s="32" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>655</v>
+        <v>609</v>
       </c>
       <c r="B76" s="20" t="s">
-        <v>695</v>
+        <v>705</v>
       </c>
       <c r="C76" s="20" t="s">
         <v>578</v>
       </c>
+      <c r="D76" s="14"/>
       <c r="E76" s="20" t="s">
         <v>579</v>
       </c>
@@ -16949,26 +17592,38 @@
       </c>
       <c r="L76" s="20"/>
       <c r="M76" s="20" t="s">
-        <v>885</v>
+        <v>895</v>
       </c>
       <c r="N76" s="20"/>
       <c r="O76" s="20" t="s">
-        <v>765</v>
+        <v>775</v>
       </c>
       <c r="P76" s="20" t="s">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="77" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>835</v>
+      </c>
+      <c r="Q76" s="65" t="s">
+        <v>988</v>
+      </c>
+      <c r="R76" s="65" t="s">
+        <v>1059</v>
+      </c>
+      <c r="S76" s="65"/>
+      <c r="T76" s="65"/>
+      <c r="U76" s="65"/>
+      <c r="V76" s="65"/>
+      <c r="W76" s="65"/>
+    </row>
+    <row r="77" spans="1:23" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>656</v>
+        <v>610</v>
       </c>
       <c r="B77" s="20" t="s">
-        <v>696</v>
+        <v>706</v>
       </c>
       <c r="C77" s="20" t="s">
         <v>578</v>
       </c>
+      <c r="D77" s="14"/>
       <c r="E77" s="20" t="s">
         <v>579</v>
       </c>
@@ -16988,26 +17643,38 @@
       </c>
       <c r="L77" s="20"/>
       <c r="M77" s="20" t="s">
-        <v>886</v>
+        <v>896</v>
       </c>
       <c r="N77" s="20"/>
       <c r="O77" s="20" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="P77" s="20" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="78" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>836</v>
+      </c>
+      <c r="Q77" s="65" t="s">
+        <v>989</v>
+      </c>
+      <c r="R77" s="65" t="s">
+        <v>1060</v>
+      </c>
+      <c r="S77" s="65"/>
+      <c r="T77" s="65"/>
+      <c r="U77" s="65"/>
+      <c r="V77" s="65"/>
+      <c r="W77" s="65"/>
+    </row>
+    <row r="78" spans="1:23" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>657</v>
+        <v>611</v>
       </c>
       <c r="B78" s="20" t="s">
-        <v>697</v>
+        <v>707</v>
       </c>
       <c r="C78" s="20" t="s">
         <v>578</v>
       </c>
+      <c r="D78" s="14"/>
       <c r="E78" s="20" t="s">
         <v>579</v>
       </c>
@@ -17027,22 +17694,33 @@
       </c>
       <c r="L78" s="20"/>
       <c r="M78" s="20" t="s">
-        <v>887</v>
+        <v>897</v>
       </c>
       <c r="N78" s="20"/>
       <c r="O78" s="20" t="s">
-        <v>767</v>
+        <v>777</v>
       </c>
       <c r="P78" s="20" t="s">
-        <v>827</v>
-      </c>
+        <v>837</v>
+      </c>
+      <c r="Q78" s="65" t="s">
+        <v>990</v>
+      </c>
+      <c r="R78" s="65" t="s">
+        <v>1061</v>
+      </c>
+      <c r="S78" s="65"/>
+      <c r="T78" s="65"/>
+      <c r="U78" s="65"/>
+      <c r="V78" s="65"/>
+      <c r="W78" s="65"/>
     </row>
     <row r="79" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>658</v>
+        <v>612</v>
       </c>
       <c r="B79" s="20" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c r="C79" s="20" t="s">
         <v>578</v>
@@ -17066,22 +17744,28 @@
       </c>
       <c r="L79" s="20"/>
       <c r="M79" s="20" t="s">
-        <v>888</v>
+        <v>898</v>
       </c>
       <c r="N79" s="20"/>
       <c r="O79" s="20" t="s">
-        <v>768</v>
+        <v>778</v>
       </c>
       <c r="P79" s="20" t="s">
-        <v>828</v>
+        <v>838</v>
+      </c>
+      <c r="Q79" s="14" t="s">
+        <v>991</v>
+      </c>
+      <c r="R79" s="14" t="s">
+        <v>1062</v>
       </c>
     </row>
     <row r="80" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>603</v>
+        <v>613</v>
       </c>
       <c r="B80" s="20" t="s">
-        <v>699</v>
+        <v>709</v>
       </c>
       <c r="C80" s="20" t="s">
         <v>578</v>
@@ -17105,22 +17789,28 @@
       </c>
       <c r="L80" s="20"/>
       <c r="M80" s="20" t="s">
-        <v>889</v>
+        <v>899</v>
       </c>
       <c r="N80" s="20"/>
       <c r="O80" s="20" t="s">
-        <v>769</v>
+        <v>779</v>
       </c>
       <c r="P80" s="20" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="81" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>839</v>
+      </c>
+      <c r="Q80" s="14" t="s">
+        <v>992</v>
+      </c>
+      <c r="R80" s="14" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>604</v>
+        <v>614</v>
       </c>
       <c r="B81" s="20" t="s">
-        <v>700</v>
+        <v>710</v>
       </c>
       <c r="C81" s="20" t="s">
         <v>578</v>
@@ -17144,22 +17834,28 @@
       </c>
       <c r="L81" s="20"/>
       <c r="M81" s="20" t="s">
-        <v>890</v>
+        <v>900</v>
       </c>
       <c r="N81" s="20"/>
       <c r="O81" s="20" t="s">
-        <v>770</v>
+        <v>780</v>
       </c>
       <c r="P81" s="20" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="82" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>840</v>
+      </c>
+      <c r="Q81" s="14" t="s">
+        <v>993</v>
+      </c>
+      <c r="R81" s="14" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>605</v>
+        <v>615</v>
       </c>
       <c r="B82" s="20" t="s">
-        <v>701</v>
+        <v>711</v>
       </c>
       <c r="C82" s="20" t="s">
         <v>578</v>
@@ -17183,22 +17879,28 @@
       </c>
       <c r="L82" s="20"/>
       <c r="M82" s="20" t="s">
-        <v>891</v>
+        <v>901</v>
       </c>
       <c r="N82" s="20"/>
       <c r="O82" s="20" t="s">
-        <v>771</v>
+        <v>781</v>
       </c>
       <c r="P82" s="20" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="83" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>841</v>
+      </c>
+      <c r="Q82" s="14" t="s">
+        <v>994</v>
+      </c>
+      <c r="R82" s="14" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>606</v>
+        <v>616</v>
       </c>
       <c r="B83" s="20" t="s">
-        <v>702</v>
+        <v>712</v>
       </c>
       <c r="C83" s="20" t="s">
         <v>578</v>
@@ -17222,22 +17924,28 @@
       </c>
       <c r="L83" s="20"/>
       <c r="M83" s="20" t="s">
-        <v>892</v>
+        <v>902</v>
       </c>
       <c r="N83" s="20"/>
       <c r="O83" s="20" t="s">
-        <v>772</v>
+        <v>782</v>
       </c>
       <c r="P83" s="20" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="84" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>842</v>
+      </c>
+      <c r="Q83" s="14" t="s">
+        <v>995</v>
+      </c>
+      <c r="R83" s="14" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>607</v>
+        <v>617</v>
       </c>
       <c r="B84" s="20" t="s">
-        <v>703</v>
+        <v>713</v>
       </c>
       <c r="C84" s="20" t="s">
         <v>578</v>
@@ -17261,27 +17969,32 @@
       </c>
       <c r="L84" s="20"/>
       <c r="M84" s="20" t="s">
-        <v>893</v>
+        <v>903</v>
       </c>
       <c r="N84" s="20"/>
       <c r="O84" s="20" t="s">
-        <v>773</v>
+        <v>783</v>
       </c>
       <c r="P84" s="20" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="85" spans="1:23" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>843</v>
+      </c>
+      <c r="Q84" s="14" t="s">
+        <v>996</v>
+      </c>
+      <c r="R84" s="14" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>608</v>
+        <v>618</v>
       </c>
       <c r="B85" s="20" t="s">
-        <v>704</v>
+        <v>714</v>
       </c>
       <c r="C85" s="20" t="s">
         <v>578</v>
       </c>
-      <c r="D85" s="14"/>
       <c r="E85" s="20" t="s">
         <v>579</v>
       </c>
@@ -17301,27 +18014,32 @@
       </c>
       <c r="L85" s="20"/>
       <c r="M85" s="20" t="s">
-        <v>894</v>
+        <v>904</v>
       </c>
       <c r="N85" s="20"/>
       <c r="O85" s="20" t="s">
-        <v>774</v>
+        <v>784</v>
       </c>
       <c r="P85" s="20" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="86" spans="1:23" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>844</v>
+      </c>
+      <c r="Q85" s="14" t="s">
+        <v>997</v>
+      </c>
+      <c r="R85" s="14" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>609</v>
+        <v>619</v>
       </c>
       <c r="B86" s="20" t="s">
-        <v>705</v>
+        <v>715</v>
       </c>
       <c r="C86" s="20" t="s">
         <v>578</v>
       </c>
-      <c r="D86" s="14"/>
       <c r="E86" s="20" t="s">
         <v>579</v>
       </c>
@@ -17341,34 +18059,32 @@
       </c>
       <c r="L86" s="20"/>
       <c r="M86" s="20" t="s">
-        <v>895</v>
+        <v>905</v>
       </c>
       <c r="N86" s="20"/>
       <c r="O86" s="20" t="s">
-        <v>775</v>
+        <v>785</v>
       </c>
       <c r="P86" s="20" t="s">
-        <v>835</v>
-      </c>
-      <c r="Q86" s="65"/>
-      <c r="R86" s="65"/>
-      <c r="S86" s="65"/>
-      <c r="T86" s="65"/>
-      <c r="U86" s="65"/>
-      <c r="V86" s="65"/>
-      <c r="W86" s="65"/>
-    </row>
-    <row r="87" spans="1:23" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>845</v>
+      </c>
+      <c r="Q86" s="14" t="s">
+        <v>998</v>
+      </c>
+      <c r="R86" s="14" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="B87" s="20" t="s">
-        <v>706</v>
+        <v>716</v>
       </c>
       <c r="C87" s="20" t="s">
         <v>578</v>
       </c>
-      <c r="D87" s="14"/>
       <c r="E87" s="20" t="s">
         <v>579</v>
       </c>
@@ -17388,34 +18104,32 @@
       </c>
       <c r="L87" s="20"/>
       <c r="M87" s="20" t="s">
-        <v>896</v>
+        <v>906</v>
       </c>
       <c r="N87" s="20"/>
       <c r="O87" s="20" t="s">
-        <v>776</v>
+        <v>786</v>
       </c>
       <c r="P87" s="20" t="s">
-        <v>836</v>
-      </c>
-      <c r="Q87" s="65"/>
-      <c r="R87" s="65"/>
-      <c r="S87" s="65"/>
-      <c r="T87" s="65"/>
-      <c r="U87" s="65"/>
-      <c r="V87" s="65"/>
-      <c r="W87" s="65"/>
-    </row>
-    <row r="88" spans="1:23" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>846</v>
+      </c>
+      <c r="Q87" s="14" t="s">
+        <v>999</v>
+      </c>
+      <c r="R87" s="14" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>611</v>
+        <v>621</v>
       </c>
       <c r="B88" s="20" t="s">
-        <v>707</v>
+        <v>717</v>
       </c>
       <c r="C88" s="20" t="s">
         <v>578</v>
       </c>
-      <c r="D88" s="14"/>
       <c r="E88" s="20" t="s">
         <v>579</v>
       </c>
@@ -17435,29 +18149,28 @@
       </c>
       <c r="L88" s="20"/>
       <c r="M88" s="20" t="s">
-        <v>897</v>
+        <v>907</v>
       </c>
       <c r="N88" s="20"/>
       <c r="O88" s="20" t="s">
-        <v>777</v>
+        <v>787</v>
       </c>
       <c r="P88" s="20" t="s">
-        <v>837</v>
-      </c>
-      <c r="Q88" s="65"/>
-      <c r="R88" s="65"/>
-      <c r="S88" s="65"/>
-      <c r="T88" s="65"/>
-      <c r="U88" s="65"/>
-      <c r="V88" s="65"/>
-      <c r="W88" s="65"/>
-    </row>
-    <row r="89" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>847</v>
+      </c>
+      <c r="Q88" s="14" t="s">
+        <v>1000</v>
+      </c>
+      <c r="R88" s="14" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B89" s="20" t="s">
-        <v>708</v>
+        <v>718</v>
       </c>
       <c r="C89" s="20" t="s">
         <v>578</v>
@@ -17481,22 +18194,28 @@
       </c>
       <c r="L89" s="20"/>
       <c r="M89" s="20" t="s">
-        <v>898</v>
+        <v>908</v>
       </c>
       <c r="N89" s="20"/>
       <c r="O89" s="20" t="s">
-        <v>778</v>
+        <v>788</v>
       </c>
       <c r="P89" s="20" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="90" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>848</v>
+      </c>
+      <c r="Q89" s="14" t="s">
+        <v>1001</v>
+      </c>
+      <c r="R89" s="14" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>613</v>
+        <v>623</v>
       </c>
       <c r="B90" s="20" t="s">
-        <v>709</v>
+        <v>719</v>
       </c>
       <c r="C90" s="20" t="s">
         <v>578</v>
@@ -17520,22 +18239,28 @@
       </c>
       <c r="L90" s="20"/>
       <c r="M90" s="20" t="s">
-        <v>899</v>
+        <v>909</v>
       </c>
       <c r="N90" s="20"/>
       <c r="O90" s="20" t="s">
-        <v>779</v>
+        <v>789</v>
       </c>
       <c r="P90" s="20" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="91" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>849</v>
+      </c>
+      <c r="Q90" s="14" t="s">
+        <v>1002</v>
+      </c>
+      <c r="R90" s="14" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>614</v>
+        <v>624</v>
       </c>
       <c r="B91" s="20" t="s">
-        <v>710</v>
+        <v>720</v>
       </c>
       <c r="C91" s="20" t="s">
         <v>578</v>
@@ -17559,22 +18284,28 @@
       </c>
       <c r="L91" s="20"/>
       <c r="M91" s="20" t="s">
-        <v>900</v>
+        <v>910</v>
       </c>
       <c r="N91" s="20"/>
       <c r="O91" s="20" t="s">
-        <v>780</v>
+        <v>790</v>
       </c>
       <c r="P91" s="20" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="92" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>850</v>
+      </c>
+      <c r="Q91" s="14" t="s">
+        <v>1003</v>
+      </c>
+      <c r="R91" s="14" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>615</v>
+        <v>625</v>
       </c>
       <c r="B92" s="20" t="s">
-        <v>711</v>
+        <v>721</v>
       </c>
       <c r="C92" s="20" t="s">
         <v>578</v>
@@ -17598,22 +18329,28 @@
       </c>
       <c r="L92" s="20"/>
       <c r="M92" s="20" t="s">
-        <v>901</v>
+        <v>911</v>
       </c>
       <c r="N92" s="20"/>
       <c r="O92" s="20" t="s">
-        <v>781</v>
+        <v>791</v>
       </c>
       <c r="P92" s="20" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="93" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>851</v>
+      </c>
+      <c r="Q92" s="14" t="s">
+        <v>1004</v>
+      </c>
+      <c r="R92" s="14" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>616</v>
+        <v>626</v>
       </c>
       <c r="B93" s="20" t="s">
-        <v>712</v>
+        <v>722</v>
       </c>
       <c r="C93" s="20" t="s">
         <v>578</v>
@@ -17637,22 +18374,28 @@
       </c>
       <c r="L93" s="20"/>
       <c r="M93" s="20" t="s">
-        <v>902</v>
+        <v>912</v>
       </c>
       <c r="N93" s="20"/>
       <c r="O93" s="20" t="s">
-        <v>782</v>
+        <v>792</v>
       </c>
       <c r="P93" s="20" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="94" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>852</v>
+      </c>
+      <c r="Q93" s="14" t="s">
+        <v>1005</v>
+      </c>
+      <c r="R93" s="14" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>617</v>
+        <v>583</v>
       </c>
       <c r="B94" s="20" t="s">
-        <v>713</v>
+        <v>593</v>
       </c>
       <c r="C94" s="20" t="s">
         <v>578</v>
@@ -17676,22 +18419,28 @@
       </c>
       <c r="L94" s="20"/>
       <c r="M94" s="20" t="s">
-        <v>903</v>
+        <v>913</v>
       </c>
       <c r="N94" s="20"/>
       <c r="O94" s="20" t="s">
-        <v>783</v>
+        <v>935</v>
       </c>
       <c r="P94" s="20" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="95" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>925</v>
+      </c>
+      <c r="Q94" s="14" t="s">
+        <v>1008</v>
+      </c>
+      <c r="R94" s="14" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>618</v>
+        <v>584</v>
       </c>
       <c r="B95" s="20" t="s">
-        <v>714</v>
+        <v>594</v>
       </c>
       <c r="C95" s="20" t="s">
         <v>578</v>
@@ -17715,22 +18464,28 @@
       </c>
       <c r="L95" s="20"/>
       <c r="M95" s="20" t="s">
-        <v>904</v>
+        <v>914</v>
       </c>
       <c r="N95" s="20"/>
       <c r="O95" s="20" t="s">
-        <v>784</v>
+        <v>936</v>
       </c>
       <c r="P95" s="20" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="96" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+        <v>926</v>
+      </c>
+      <c r="Q95" s="14" t="s">
+        <v>1009</v>
+      </c>
+      <c r="R95" s="14" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>619</v>
+        <v>585</v>
       </c>
       <c r="B96" s="20" t="s">
-        <v>715</v>
+        <v>595</v>
       </c>
       <c r="C96" s="20" t="s">
         <v>578</v>
@@ -17754,22 +18509,28 @@
       </c>
       <c r="L96" s="20"/>
       <c r="M96" s="20" t="s">
-        <v>905</v>
+        <v>915</v>
       </c>
       <c r="N96" s="20"/>
       <c r="O96" s="20" t="s">
-        <v>785</v>
+        <v>937</v>
       </c>
       <c r="P96" s="20" t="s">
-        <v>845</v>
+        <v>927</v>
+      </c>
+      <c r="Q96" s="14" t="s">
+        <v>1010</v>
+      </c>
+      <c r="R96" s="14" t="s">
+        <v>1079</v>
       </c>
     </row>
     <row r="97" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>620</v>
+        <v>586</v>
       </c>
       <c r="B97" s="20" t="s">
-        <v>716</v>
+        <v>596</v>
       </c>
       <c r="C97" s="20" t="s">
         <v>578</v>
@@ -17793,22 +18554,28 @@
       </c>
       <c r="L97" s="20"/>
       <c r="M97" s="20" t="s">
-        <v>906</v>
+        <v>916</v>
       </c>
       <c r="N97" s="20"/>
       <c r="O97" s="20" t="s">
-        <v>786</v>
+        <v>938</v>
       </c>
       <c r="P97" s="20" t="s">
-        <v>846</v>
+        <v>928</v>
+      </c>
+      <c r="Q97" s="14" t="s">
+        <v>1011</v>
+      </c>
+      <c r="R97" s="14" t="s">
+        <v>1080</v>
       </c>
     </row>
     <row r="98" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>621</v>
+        <v>587</v>
       </c>
       <c r="B98" s="20" t="s">
-        <v>717</v>
+        <v>597</v>
       </c>
       <c r="C98" s="20" t="s">
         <v>578</v>
@@ -17832,22 +18599,28 @@
       </c>
       <c r="L98" s="20"/>
       <c r="M98" s="20" t="s">
-        <v>907</v>
+        <v>917</v>
       </c>
       <c r="N98" s="20"/>
       <c r="O98" s="20" t="s">
-        <v>787</v>
+        <v>939</v>
       </c>
       <c r="P98" s="20" t="s">
-        <v>847</v>
+        <v>929</v>
+      </c>
+      <c r="Q98" s="14" t="s">
+        <v>1012</v>
+      </c>
+      <c r="R98" s="14" t="s">
+        <v>1081</v>
       </c>
     </row>
     <row r="99" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>622</v>
+        <v>588</v>
       </c>
       <c r="B99" s="20" t="s">
-        <v>718</v>
+        <v>598</v>
       </c>
       <c r="C99" s="20" t="s">
         <v>578</v>
@@ -17871,22 +18644,28 @@
       </c>
       <c r="L99" s="20"/>
       <c r="M99" s="20" t="s">
-        <v>908</v>
+        <v>918</v>
       </c>
       <c r="N99" s="20"/>
       <c r="O99" s="20" t="s">
-        <v>788</v>
+        <v>940</v>
       </c>
       <c r="P99" s="20" t="s">
-        <v>848</v>
+        <v>930</v>
+      </c>
+      <c r="Q99" s="14" t="s">
+        <v>1013</v>
+      </c>
+      <c r="R99" s="14" t="s">
+        <v>1082</v>
       </c>
     </row>
     <row r="100" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>623</v>
+        <v>589</v>
       </c>
       <c r="B100" s="20" t="s">
-        <v>719</v>
+        <v>599</v>
       </c>
       <c r="C100" s="20" t="s">
         <v>578</v>
@@ -17910,22 +18689,28 @@
       </c>
       <c r="L100" s="20"/>
       <c r="M100" s="20" t="s">
-        <v>909</v>
+        <v>919</v>
       </c>
       <c r="N100" s="20"/>
       <c r="O100" s="20" t="s">
-        <v>789</v>
+        <v>941</v>
       </c>
       <c r="P100" s="20" t="s">
-        <v>849</v>
+        <v>931</v>
+      </c>
+      <c r="Q100" s="14" t="s">
+        <v>1014</v>
+      </c>
+      <c r="R100" s="14" t="s">
+        <v>1083</v>
       </c>
     </row>
     <row r="101" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>624</v>
+        <v>590</v>
       </c>
       <c r="B101" s="20" t="s">
-        <v>720</v>
+        <v>600</v>
       </c>
       <c r="C101" s="20" t="s">
         <v>578</v>
@@ -17949,22 +18734,28 @@
       </c>
       <c r="L101" s="20"/>
       <c r="M101" s="20" t="s">
-        <v>910</v>
+        <v>920</v>
       </c>
       <c r="N101" s="20"/>
       <c r="O101" s="20" t="s">
-        <v>790</v>
+        <v>942</v>
       </c>
       <c r="P101" s="20" t="s">
-        <v>850</v>
+        <v>932</v>
+      </c>
+      <c r="Q101" s="14" t="s">
+        <v>1015</v>
+      </c>
+      <c r="R101" s="14" t="s">
+        <v>1084</v>
       </c>
     </row>
     <row r="102" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>625</v>
+        <v>591</v>
       </c>
       <c r="B102" s="20" t="s">
-        <v>721</v>
+        <v>601</v>
       </c>
       <c r="C102" s="20" t="s">
         <v>578</v>
@@ -17988,22 +18779,28 @@
       </c>
       <c r="L102" s="20"/>
       <c r="M102" s="20" t="s">
-        <v>911</v>
+        <v>921</v>
       </c>
       <c r="N102" s="20"/>
       <c r="O102" s="20" t="s">
-        <v>791</v>
+        <v>943</v>
       </c>
       <c r="P102" s="20" t="s">
-        <v>851</v>
+        <v>933</v>
+      </c>
+      <c r="Q102" s="14" t="s">
+        <v>1016</v>
+      </c>
+      <c r="R102" s="14" t="s">
+        <v>1085</v>
       </c>
     </row>
     <row r="103" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>626</v>
+        <v>592</v>
       </c>
       <c r="B103" s="20" t="s">
-        <v>722</v>
+        <v>602</v>
       </c>
       <c r="C103" s="20" t="s">
         <v>578</v>
@@ -18027,14 +18824,20 @@
       </c>
       <c r="L103" s="20"/>
       <c r="M103" s="20" t="s">
-        <v>912</v>
+        <v>922</v>
       </c>
       <c r="N103" s="20"/>
       <c r="O103" s="20" t="s">
-        <v>792</v>
+        <v>944</v>
       </c>
       <c r="P103" s="20" t="s">
-        <v>852</v>
+        <v>934</v>
+      </c>
+      <c r="Q103" s="14" t="s">
+        <v>1017</v>
+      </c>
+      <c r="R103" s="14" t="s">
+        <v>1086</v>
       </c>
     </row>
     <row r="104" spans="1:23" x14ac:dyDescent="0.25">
@@ -18539,610 +19342,610 @@
     </row>
     <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126" s="20" t="s">
-        <v>935</v>
+        <v>733</v>
       </c>
       <c r="B126" s="20" t="s">
-        <v>925</v>
+        <v>793</v>
       </c>
     </row>
     <row r="127" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A127" s="20" t="s">
-        <v>936</v>
+        <v>734</v>
       </c>
       <c r="B127" s="20" t="s">
-        <v>926</v>
+        <v>794</v>
       </c>
     </row>
     <row r="128" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A128" s="20" t="s">
-        <v>937</v>
+        <v>735</v>
       </c>
       <c r="B128" s="20" t="s">
-        <v>927</v>
+        <v>795</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="20" t="s">
-        <v>938</v>
+        <v>736</v>
       </c>
       <c r="B129" s="20" t="s">
-        <v>928</v>
+        <v>796</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="20" t="s">
-        <v>939</v>
+        <v>737</v>
       </c>
       <c r="B130" s="20" t="s">
-        <v>929</v>
+        <v>797</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="20" t="s">
-        <v>940</v>
+        <v>738</v>
       </c>
       <c r="B131" s="20" t="s">
-        <v>930</v>
+        <v>798</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="20" t="s">
-        <v>941</v>
+        <v>739</v>
       </c>
       <c r="B132" s="20" t="s">
-        <v>931</v>
+        <v>799</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="20" t="s">
-        <v>942</v>
+        <v>740</v>
       </c>
       <c r="B133" s="20" t="s">
-        <v>932</v>
+        <v>800</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="20" t="s">
-        <v>943</v>
+        <v>741</v>
       </c>
       <c r="B134" s="20" t="s">
-        <v>933</v>
+        <v>801</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="20" t="s">
-        <v>944</v>
+        <v>742</v>
       </c>
       <c r="B135" s="20" t="s">
-        <v>934</v>
+        <v>802</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="20" t="s">
-        <v>733</v>
+        <v>743</v>
       </c>
       <c r="B136" s="20" t="s">
-        <v>793</v>
+        <v>803</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="20" t="s">
-        <v>734</v>
+        <v>744</v>
       </c>
       <c r="B137" s="20" t="s">
-        <v>794</v>
+        <v>804</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="20" t="s">
-        <v>735</v>
+        <v>745</v>
       </c>
       <c r="B138" s="20" t="s">
-        <v>795</v>
+        <v>805</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="20" t="s">
-        <v>736</v>
+        <v>746</v>
       </c>
       <c r="B139" s="20" t="s">
-        <v>796</v>
+        <v>806</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="20" t="s">
-        <v>737</v>
+        <v>747</v>
       </c>
       <c r="B140" s="20" t="s">
-        <v>797</v>
+        <v>807</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="20" t="s">
-        <v>738</v>
+        <v>748</v>
       </c>
       <c r="B141" s="20" t="s">
-        <v>798</v>
+        <v>808</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="20" t="s">
-        <v>739</v>
+        <v>749</v>
       </c>
       <c r="B142" s="20" t="s">
-        <v>799</v>
+        <v>809</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="20" t="s">
-        <v>740</v>
+        <v>750</v>
       </c>
       <c r="B143" s="20" t="s">
-        <v>800</v>
+        <v>810</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="20" t="s">
-        <v>741</v>
+        <v>751</v>
       </c>
       <c r="B144" s="20" t="s">
-        <v>801</v>
+        <v>811</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="20" t="s">
-        <v>742</v>
+        <v>752</v>
       </c>
       <c r="B145" s="20" t="s">
-        <v>802</v>
+        <v>812</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="20" t="s">
-        <v>743</v>
+        <v>753</v>
       </c>
       <c r="B146" s="20" t="s">
-        <v>803</v>
+        <v>813</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="20" t="s">
-        <v>744</v>
+        <v>754</v>
       </c>
       <c r="B147" s="20" t="s">
-        <v>804</v>
+        <v>814</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="20" t="s">
-        <v>745</v>
+        <v>755</v>
       </c>
       <c r="B148" s="20" t="s">
-        <v>805</v>
+        <v>815</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="20" t="s">
-        <v>746</v>
+        <v>756</v>
       </c>
       <c r="B149" s="20" t="s">
-        <v>806</v>
+        <v>816</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="20" t="s">
-        <v>747</v>
+        <v>757</v>
       </c>
       <c r="B150" s="20" t="s">
-        <v>807</v>
+        <v>817</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="20" t="s">
-        <v>748</v>
+        <v>758</v>
       </c>
       <c r="B151" s="20" t="s">
-        <v>808</v>
+        <v>818</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="20" t="s">
-        <v>749</v>
+        <v>759</v>
       </c>
       <c r="B152" s="20" t="s">
-        <v>809</v>
+        <v>819</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="20" t="s">
-        <v>750</v>
+        <v>760</v>
       </c>
       <c r="B153" s="20" t="s">
-        <v>810</v>
+        <v>820</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="20" t="s">
-        <v>751</v>
+        <v>761</v>
       </c>
       <c r="B154" s="20" t="s">
-        <v>811</v>
+        <v>821</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="20" t="s">
-        <v>752</v>
+        <v>762</v>
       </c>
       <c r="B155" s="20" t="s">
-        <v>812</v>
+        <v>822</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="20" t="s">
-        <v>753</v>
+        <v>763</v>
       </c>
       <c r="B156" s="20" t="s">
-        <v>813</v>
+        <v>823</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="20" t="s">
-        <v>754</v>
+        <v>764</v>
       </c>
       <c r="B157" s="20" t="s">
-        <v>814</v>
+        <v>824</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="20" t="s">
-        <v>755</v>
+        <v>765</v>
       </c>
       <c r="B158" s="20" t="s">
-        <v>815</v>
+        <v>825</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="20" t="s">
-        <v>756</v>
+        <v>766</v>
       </c>
       <c r="B159" s="20" t="s">
-        <v>816</v>
+        <v>826</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="20" t="s">
-        <v>757</v>
+        <v>767</v>
       </c>
       <c r="B160" s="20" t="s">
-        <v>817</v>
+        <v>827</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="20" t="s">
-        <v>758</v>
+        <v>768</v>
       </c>
       <c r="B161" s="20" t="s">
-        <v>818</v>
+        <v>828</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="20" t="s">
-        <v>759</v>
+        <v>769</v>
       </c>
       <c r="B162" s="20" t="s">
-        <v>819</v>
+        <v>829</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="20" t="s">
-        <v>760</v>
+        <v>770</v>
       </c>
       <c r="B163" s="20" t="s">
-        <v>820</v>
+        <v>830</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="20" t="s">
-        <v>761</v>
+        <v>771</v>
       </c>
       <c r="B164" s="20" t="s">
-        <v>821</v>
+        <v>831</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="20" t="s">
-        <v>762</v>
+        <v>772</v>
       </c>
       <c r="B165" s="20" t="s">
-        <v>822</v>
+        <v>832</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="20" t="s">
-        <v>763</v>
+        <v>773</v>
       </c>
       <c r="B166" s="20" t="s">
-        <v>823</v>
+        <v>833</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="20" t="s">
-        <v>764</v>
+        <v>774</v>
       </c>
       <c r="B167" s="20" t="s">
-        <v>824</v>
+        <v>834</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="20" t="s">
-        <v>765</v>
+        <v>775</v>
       </c>
       <c r="B168" s="20" t="s">
-        <v>825</v>
+        <v>835</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="20" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="B169" s="20" t="s">
-        <v>826</v>
+        <v>836</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="20" t="s">
-        <v>767</v>
+        <v>777</v>
       </c>
       <c r="B170" s="20" t="s">
-        <v>827</v>
+        <v>837</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="20" t="s">
-        <v>768</v>
+        <v>778</v>
       </c>
       <c r="B171" s="20" t="s">
-        <v>828</v>
+        <v>838</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="20" t="s">
-        <v>769</v>
+        <v>779</v>
       </c>
       <c r="B172" s="20" t="s">
-        <v>829</v>
+        <v>839</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="20" t="s">
-        <v>770</v>
+        <v>780</v>
       </c>
       <c r="B173" s="20" t="s">
-        <v>830</v>
+        <v>840</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="20" t="s">
-        <v>771</v>
+        <v>781</v>
       </c>
       <c r="B174" s="20" t="s">
-        <v>831</v>
+        <v>841</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="20" t="s">
-        <v>772</v>
+        <v>782</v>
       </c>
       <c r="B175" s="20" t="s">
-        <v>832</v>
+        <v>842</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="20" t="s">
-        <v>773</v>
+        <v>783</v>
       </c>
       <c r="B176" s="20" t="s">
-        <v>833</v>
+        <v>843</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="20" t="s">
-        <v>774</v>
+        <v>784</v>
       </c>
       <c r="B177" s="20" t="s">
-        <v>834</v>
+        <v>844</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="20" t="s">
-        <v>775</v>
+        <v>785</v>
       </c>
       <c r="B178" s="20" t="s">
-        <v>835</v>
+        <v>845</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="20" t="s">
-        <v>776</v>
+        <v>786</v>
       </c>
       <c r="B179" s="20" t="s">
-        <v>836</v>
+        <v>846</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="20" t="s">
-        <v>777</v>
+        <v>787</v>
       </c>
       <c r="B180" s="20" t="s">
-        <v>837</v>
+        <v>847</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="20" t="s">
-        <v>778</v>
+        <v>788</v>
       </c>
       <c r="B181" s="20" t="s">
-        <v>838</v>
+        <v>848</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="20" t="s">
-        <v>779</v>
+        <v>789</v>
       </c>
       <c r="B182" s="20" t="s">
-        <v>839</v>
+        <v>849</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="20" t="s">
-        <v>780</v>
+        <v>790</v>
       </c>
       <c r="B183" s="20" t="s">
-        <v>840</v>
+        <v>850</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="20" t="s">
-        <v>781</v>
+        <v>791</v>
       </c>
       <c r="B184" s="20" t="s">
-        <v>841</v>
+        <v>851</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="20" t="s">
-        <v>782</v>
+        <v>792</v>
       </c>
       <c r="B185" s="20" t="s">
-        <v>842</v>
+        <v>852</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="20" t="s">
-        <v>783</v>
+        <v>935</v>
       </c>
       <c r="B186" s="20" t="s">
-        <v>843</v>
+        <v>925</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="20" t="s">
-        <v>784</v>
+        <v>936</v>
       </c>
       <c r="B187" s="20" t="s">
-        <v>844</v>
+        <v>926</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="20" t="s">
-        <v>785</v>
+        <v>937</v>
       </c>
       <c r="B188" s="20" t="s">
-        <v>845</v>
+        <v>927</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="20" t="s">
-        <v>786</v>
+        <v>938</v>
       </c>
       <c r="B189" s="20" t="s">
-        <v>846</v>
+        <v>928</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="20" t="s">
-        <v>787</v>
+        <v>939</v>
       </c>
       <c r="B190" s="20" t="s">
-        <v>847</v>
+        <v>929</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="20" t="s">
-        <v>788</v>
+        <v>940</v>
       </c>
       <c r="B191" s="20" t="s">
-        <v>848</v>
+        <v>930</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="20" t="s">
-        <v>789</v>
+        <v>941</v>
       </c>
       <c r="B192" s="20" t="s">
-        <v>849</v>
+        <v>931</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="20" t="s">
-        <v>790</v>
+        <v>942</v>
       </c>
       <c r="B193" s="20" t="s">
-        <v>850</v>
+        <v>932</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="20" t="s">
-        <v>791</v>
+        <v>943</v>
       </c>
       <c r="B194" s="20" t="s">
-        <v>851</v>
+        <v>933</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="20" t="s">
-        <v>792</v>
+        <v>944</v>
       </c>
       <c r="B195" s="20" t="s">
-        <v>852</v>
+        <v>934</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0"/>
-  <conditionalFormatting sqref="A56:A61 A34:A43">
-    <cfRule type="duplicateValues" dxfId="23" priority="59"/>
+  <conditionalFormatting sqref="A94:A103 A46:A51">
+    <cfRule type="duplicateValues" dxfId="20" priority="59"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A136:B195">
-    <cfRule type="duplicateValues" dxfId="21" priority="3"/>
+  <conditionalFormatting sqref="A186:B186">
+    <cfRule type="duplicateValues" dxfId="19" priority="60"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A196:XFD1048576 A79:A103 X104:XFD126 X90:XFD90 C126:W126 Q91:XFD103 C127:XFD195">
-    <cfRule type="duplicateValues" dxfId="20" priority="34"/>
+  <conditionalFormatting sqref="A187:B195">
+    <cfRule type="duplicateValues" dxfId="18" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A126:B185">
+    <cfRule type="duplicateValues" dxfId="17" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A196:XFD1048576 A69:A93 X104:XFD125 C126:XFD195 X80:XFD80 Q81:XFD93">
+    <cfRule type="duplicateValues" dxfId="16" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B27 B11:B15">
-    <cfRule type="duplicateValues" dxfId="19" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="39"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B34:B61">
-    <cfRule type="duplicateValues" dxfId="18" priority="36"/>
+  <conditionalFormatting sqref="B34:B51 B94:B103">
+    <cfRule type="duplicateValues" dxfId="14" priority="36"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B62:B79">
-    <cfRule type="duplicateValues" dxfId="17" priority="16"/>
+  <conditionalFormatting sqref="B52:B69">
+    <cfRule type="duplicateValues" dxfId="13" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B80:B85">
-    <cfRule type="duplicateValues" dxfId="16" priority="15"/>
+  <conditionalFormatting sqref="B70:B75">
+    <cfRule type="duplicateValues" dxfId="12" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B86:B91">
-    <cfRule type="duplicateValues" dxfId="15" priority="14"/>
+  <conditionalFormatting sqref="B76:B81">
+    <cfRule type="duplicateValues" dxfId="11" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B92:B97">
-    <cfRule type="duplicateValues" dxfId="14" priority="13"/>
+  <conditionalFormatting sqref="B82:B87">
+    <cfRule type="duplicateValues" dxfId="10" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B98:B103">
-    <cfRule type="duplicateValues" dxfId="13" priority="12"/>
+  <conditionalFormatting sqref="B88:B93">
+    <cfRule type="duplicateValues" dxfId="9" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B106:B112 B114:B119">
-    <cfRule type="duplicateValues" dxfId="12" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="40"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O35:P103">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+  <conditionalFormatting sqref="O94:XFD94 Q34:XFD57 Q95:XFD103">
+    <cfRule type="duplicateValues" dxfId="7" priority="35"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O34:XFD34 Q35:XFD67">
-    <cfRule type="duplicateValues" dxfId="10" priority="35"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A127:B135">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A126:B126">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="O34:P93 O95:P103">
+    <cfRule type="duplicateValues" dxfId="6" priority="72"/>
   </conditionalFormatting>
   <dataValidations count="15">
     <dataValidation type="textLength" errorStyle="information" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Your summary seems too short!" error="Please provide a thorough description of the goals and objectives of this study.  A working abstract from the associated manuscript may be suitable.  Include as much text as necessary." prompt="Please provide a thorough description of the goals and objectives of this study.  A working abstract from the associated manuscript may be suitable.  Include as much text as necessary." sqref="B12" xr:uid="{6DD1BA29-F299-4D8E-AF94-669CA4660371}">
@@ -19265,10 +20068,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F7:F12">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13:F18">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="Each sample title should be unique. _x000a_Use biol/tech rep numbers (when _x000a_applicable) to unique the titles. _x000a_For example:_x000a_Muscle, exercised, 60min, biol rep1_x000a_Muscle, exercised, 60min, biol rep2_x000a_" sqref="F7:F18" xr:uid="{E1213116-0C92-4E16-8A25-FA0D7A7C18E0}"/>
@@ -19344,7 +20147,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A9:G1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -26232,13 +27035,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="vq7Iatnd+jE8zxfc8RHY55fRB2dEGEJ3skZO89caxOF1BDbSneErENA/VUKxyZa97CW266clRXMnwj+vpKgg4g==" saltValue="+ZFTuxJiYJiRThwP1ksobg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <conditionalFormatting sqref="A61:E69">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:Y31">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T26:Y31">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from the drop down menu" sqref="I30:K32" xr:uid="{79D6ECAE-44AD-41AB-84C9-88F44BE0AE81}">

</xml_diff>